<commit_message>
Updated error codes and test procedure for Resideo Software
</commit_message>
<xml_diff>
--- a/NI-2010/Drivers/Resideo Gas Valve/Documentation/Copy of WV8860H Error Code mappings.xlsx
+++ b/NI-2010/Drivers/Resideo Gas Valve/Documentation/Copy of WV8860H Error Code mappings.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\205841\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Drivers\Resideo Gas Valve\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925373E2-4BB3-46B4-AA92-28EB1837E045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5400FC-D61D-41C7-AF05-C3EB7149AD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E2586048-5F2F-40A6-9DF0-A1115D418CEC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E2586048-5F2F-40A6-9DF0-A1115D418CEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="171">
   <si>
     <t>MVOpen</t>
   </si>
@@ -331,12 +332,6 @@
   </si>
   <si>
     <t>Brief Description (I don’t fully understand some of the abbreviations)</t>
-  </si>
-  <si>
-    <t>Heat</t>
-  </si>
-  <si>
-    <t>Ambient</t>
   </si>
   <si>
     <t>Thermowell Rate</t>
@@ -477,6 +472,150 @@
   </si>
   <si>
     <t>Y (system shutdown) (fatal error)</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>How to Check</t>
+  </si>
+  <si>
+    <t>Normal Operation</t>
+  </si>
+  <si>
+    <t>Heat the tank, then do a continuous draw. It should not flash an error code</t>
+  </si>
+  <si>
+    <t>Heat the tank, do a draw, then stop. Let it heat to setpoint. No error should occur</t>
+  </si>
+  <si>
+    <t>Replace thermistor with 2kOhm resistor</t>
+  </si>
+  <si>
+    <t>Stuck thermistor in high condition. Not heating</t>
+  </si>
+  <si>
+    <t>Stuck thermistor in high condition. Heating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dangle the thermistor between the inner and outer door. </t>
+  </si>
+  <si>
+    <t>Stuck thermistor in cold condition. Heating</t>
+  </si>
+  <si>
+    <t>Place thermistor on outside of outer door. Dangle in ambient</t>
+  </si>
+  <si>
+    <t>Stuck thermistor in cold condition. Not Heating</t>
+  </si>
+  <si>
+    <t>Additional Checks</t>
+  </si>
+  <si>
+    <t>Verify reset algorithm</t>
+  </si>
+  <si>
+    <t>Induce LDO failure</t>
+  </si>
+  <si>
+    <t>Populate a BIN, then go back to cooling. Clear the bin by sending 200 deg F setpoint temp. Unit should shutdown. Then relight, bins should be clear and cylce counter reset.</t>
+  </si>
+  <si>
+    <t>ECO Temp Full Lock</t>
+  </si>
+  <si>
+    <t>Heat thermowell thermistor past 188F 5 times. Each time it passes 188, the system should shutdown. It will fire back up normally once thermowell decreases below 188. This can only happen 5 times. Then a full lock.</t>
+  </si>
+  <si>
+    <t>Run normal cycle, run for 30 minutes, populate a bin. Then run a cycle again. After 30 minutes (Heating state), remove the thermistor and allow to cool (-15F below bin). LDO should trigger. Once triggered, unit should shutdown. Relight, LDO should flash, turn knob to OFF, then relight, LDO should still flash. Reinstall, allow for a full heating cycle. It should blink read until 30 minutes. At 30 minutes, it will check, then it should flash orange. Re test, this time cut gas, do not turn to OFF. In this condition, on the second relight attempt, it should clear the error. THis is becasue we look for the knob to be put in the OFF position.</t>
+  </si>
+  <si>
+    <t>Run full LDO test</t>
+  </si>
+  <si>
+    <t>Verify shutdown before .04% AFCO</t>
+  </si>
+  <si>
+    <t>Place thermistor on outside of outer door. Dangle in ambient. Allow thermowell to dangle in ambient. Or tape solenoid pins to prevent MV from opening.</t>
+  </si>
+  <si>
+    <t>Replace thermistor with 2kOhm resistor. Remove thermowell sensor and dangle or tape MV to prevent opening.</t>
+  </si>
+  <si>
+    <t>Cycle test</t>
+  </si>
+  <si>
+    <t>Place in field and on RLT units</t>
+  </si>
+  <si>
+    <t>Dangle thermistor between the inner and outer door, and allow the thermowell temp to dangle in air, or Tape MV pins</t>
+  </si>
+  <si>
+    <t>Dangle Therimistor (Between Inner and Outer Door) - Heating</t>
+  </si>
+  <si>
+    <t>Dangle Thermistor (Between Inner and Outer Door) - Not Heating</t>
+  </si>
+  <si>
+    <t>Unplug thermowell</t>
+  </si>
+  <si>
+    <t>Chamber Sensor Failure</t>
+  </si>
+  <si>
+    <t>Unplug chamber sensor</t>
+  </si>
+  <si>
+    <t>Pilot Voltage Low</t>
+  </si>
+  <si>
+    <t>Prove pilot, then drop voltage. Maybe a power supply</t>
+  </si>
+  <si>
+    <t>Chamber Sensor Failure (WV8860 only) - Disconnected</t>
+  </si>
+  <si>
+    <t>Normal Operation - Continuous Draw</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Temperature High Limit (MV Stuck Open) - 5 Limit</t>
+  </si>
+  <si>
+    <t>Full Lockout if 5 occurances</t>
+  </si>
+  <si>
+    <t>Run normal cycle, run for 30 minutes, populate a bin. Then run a cycle again. After 30 minutes (Heating state), remove the thermistor and allow to cool (-15F below bin). LDO should trigger. Once triggered, unit should shutdown. Relight, LDO should flash, turn knob to OFF, then relight, LDO should still flash. Reinstall, allow for a full heating cycle. It should blink red until 30 minutes. At 30 minutes, it will check, then it should flash orange. Re test, this time cut gas, do not turn to OFF. In this condition, on the second relight attempt, it should clear the error. THis is becasue we look for the knob to be put in the OFF position.</t>
+  </si>
+  <si>
+    <t>Reset Algorithm</t>
+  </si>
+  <si>
+    <t>Verify 200F Reset Algorithm</t>
+  </si>
+  <si>
+    <t>System Shutdown</t>
+  </si>
+  <si>
+    <t>When a BIN is populated, send 200F setpoint in Vesta while in the cooling mode. System should clear BIN and shutdown.</t>
+  </si>
+  <si>
+    <t>Test Pass?</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Chamber Thermistor Heat Rate (Snap Short &gt;12F)</t>
+  </si>
+  <si>
+    <t>Chamber Thermistor &gt; Ambient + 50</t>
   </si>
 </sst>
 </file>
@@ -571,7 +710,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -841,11 +980,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -869,6 +1032,48 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -906,17 +1111,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1009,16 +1232,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2368826</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>164411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1847850</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1243220</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>88211</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1033,8 +1256,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7439025" y="5724525"/>
-          <a:ext cx="3352800" cy="495300"/>
+          <a:off x="4356652" y="11039476"/>
+          <a:ext cx="3355285" cy="495300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1090,16 +1313,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1410528</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>31061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2368826</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>59636</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1116,8 +1339,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6477000" y="5972175"/>
-          <a:ext cx="962025" cy="28575"/>
+          <a:off x="3398354" y="11287126"/>
+          <a:ext cx="958298" cy="28575"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1145,16 +1368,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2534479</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>41412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1847850</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2990851</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>155712</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1169,8 +1392,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7439025" y="6496050"/>
-          <a:ext cx="3352800" cy="495300"/>
+          <a:off x="9003196" y="11106977"/>
+          <a:ext cx="3355285" cy="495300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1226,16 +1449,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1544293</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>165237</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2534479</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>98562</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1252,8 +1475,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6448425" y="6619875"/>
-          <a:ext cx="990600" cy="123825"/>
+          <a:off x="8013010" y="11230802"/>
+          <a:ext cx="990186" cy="123825"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1279,13 +1502,88 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>463826</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>546652</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3282439C-CF41-E879-B965-79B969897258}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17053891" y="7296978"/>
+          <a:ext cx="3495261" cy="778565"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>To</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> clear error 9, wait for 10 seconds in pilot. Then turn back to some number for the setpoint.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1323,7 +1621,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1429,7 +1727,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1571,7 +1869,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1579,61 +1877,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26CEB2B-2FFC-4998-AD64-994C9AA677DA}">
-  <dimension ref="B1:N36"/>
+  <dimension ref="B1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B36" activeCellId="3" sqref="B32 B33 B35 B36"/>
+    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="58" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="7" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.7265625" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
-    <col min="10" max="10" width="30.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="74" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33" customWidth="1"/>
-    <col min="13" max="13" width="31.6328125" customWidth="1"/>
-    <col min="14" max="14" width="74.90625" customWidth="1"/>
+    <col min="13" max="13" width="31.5703125" customWidth="1"/>
+    <col min="14" max="14" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B2" s="20" t="s">
+    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="23"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="M2" s="26" t="s">
+      <c r="L2" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="34" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>73</v>
       </c>
@@ -1654,13 +1953,13 @@
       <c r="I3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="19"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="35"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>0</v>
       </c>
@@ -1684,22 +1983,22 @@
         <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="M4" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L4" s="30" t="s">
+      <c r="N4" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="M4" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>1</v>
       </c>
@@ -1712,7 +2011,7 @@
       <c r="F5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="19" t="s">
         <v>79</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1722,22 +2021,22 @@
         <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="M5" s="13" t="s">
+      <c r="N5" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>2</v>
       </c>
@@ -1750,7 +2049,7 @@
       <c r="F6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="19" t="s">
         <v>80</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -1760,22 +2059,22 @@
         <v>7</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>109</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>3</v>
       </c>
@@ -1788,7 +2087,7 @@
       <c r="F7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="19" t="s">
         <v>80</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1798,22 +2097,22 @@
         <v>7</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>109</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>4</v>
       </c>
@@ -1826,7 +2125,7 @@
       <c r="F8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="19" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1836,22 +2135,22 @@
         <v>7</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>109</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>5</v>
       </c>
@@ -1864,7 +2163,7 @@
       <c r="F9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="19" t="s">
         <v>82</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -1874,22 +2173,22 @@
         <v>7</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="M9" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="L9" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>109</v>
-      </c>
       <c r="N9" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>6</v>
       </c>
@@ -1902,7 +2201,7 @@
       <c r="F10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="19" t="s">
         <v>6</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1912,20 +2211,20 @@
         <v>10</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="M10" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="L10" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>109</v>
-      </c>
       <c r="N10" s="6"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>7</v>
       </c>
@@ -1948,20 +2247,20 @@
         <v>6</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>8</v>
       </c>
@@ -1984,22 +2283,22 @@
         <v>7</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>9</v>
       </c>
@@ -2022,22 +2321,22 @@
         <v>7</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M13" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="N13" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="N13" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>10</v>
       </c>
@@ -2063,22 +2362,22 @@
         <v>7</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M14" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>11</v>
       </c>
@@ -2101,22 +2400,22 @@
         <v>7</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>12</v>
       </c>
@@ -2139,22 +2438,22 @@
         <v>5</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M16" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N16" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>13</v>
       </c>
@@ -2177,22 +2476,22 @@
         <v>5</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>14</v>
       </c>
@@ -2215,22 +2514,22 @@
         <v>5</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M18" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>15</v>
       </c>
@@ -2253,22 +2552,22 @@
         <v>5</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
         <v>16</v>
       </c>
@@ -2291,22 +2590,22 @@
         <v>7</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
         <v>17</v>
       </c>
@@ -2329,22 +2628,22 @@
         <v>9</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L21" s="33" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="L21" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="N21" s="32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+      <c r="N21" s="20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
         <v>18</v>
       </c>
@@ -2367,22 +2666,22 @@
         <v>3</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L22" s="33" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="L22" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="N22" s="32" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+      <c r="N22" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>19</v>
       </c>
@@ -2405,22 +2704,22 @@
         <v>2</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L23" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M23" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N23" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7">
         <v>20</v>
       </c>
@@ -2444,36 +2743,42 @@
         <v>7</v>
       </c>
       <c r="J24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="M24" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="N24" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B28" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="G28" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="16" t="b">
         <v>1</v>
       </c>
@@ -2484,10 +2789,16 @@
         <v>1</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="b">
         <v>1</v>
       </c>
@@ -2498,25 +2809,37 @@
         <v>0</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="C31" s="34" t="b">
+      <c r="C31" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="15" t="b">
         <v>1</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B32" s="35" t="b">
+        <v>102</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G31" s="24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="23" t="b">
         <v>0</v>
       </c>
       <c r="C32" s="15" t="b">
@@ -2526,39 +2849,57 @@
         <v>1</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" s="35" t="b">
+        <v>102</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="C33" s="34" t="b">
+      <c r="C33" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="15" t="b">
         <v>1</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="C34" s="34" t="b">
+      <c r="C34" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D34" s="16" t="b">
         <v>0</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B35" s="35" t="b">
+        <v>103</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="23" t="b">
         <v>0</v>
       </c>
       <c r="C35" s="16" t="b">
@@ -2568,25 +2909,176 @@
         <v>0</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="35" t="b">
+        <v>103</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="C36" s="34" t="b">
+      <c r="C36" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D36" s="16" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>105</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+    </row>
+    <row r="38" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="47">
+        <v>1</v>
+      </c>
+      <c r="C38" s="47"/>
+      <c r="D38" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="E38" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" s="52"/>
+      <c r="G38" s="53"/>
+    </row>
+    <row r="39" spans="2:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="47">
+        <v>2</v>
+      </c>
+      <c r="C39" s="47"/>
+      <c r="D39" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="49"/>
+      <c r="G39" s="50"/>
+    </row>
+    <row r="40" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="47">
+        <v>3</v>
+      </c>
+      <c r="C40" s="47"/>
+      <c r="D40" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" s="49"/>
+      <c r="G40" s="50"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="47">
+        <v>4</v>
+      </c>
+      <c r="C41" s="47"/>
+      <c r="D41" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" s="49"/>
+      <c r="G41" s="50"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="47">
+        <v>5</v>
+      </c>
+      <c r="C42" s="47"/>
+      <c r="D42" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="E42" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" s="49"/>
+      <c r="G42" s="50"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="47">
+        <v>6</v>
+      </c>
+      <c r="C43" s="47"/>
+      <c r="D43" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="F43" s="49"/>
+      <c r="G43" s="50"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="47">
+        <v>7</v>
+      </c>
+      <c r="C44" s="47"/>
+      <c r="D44" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="F44" s="49"/>
+      <c r="G44" s="50"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="47">
+        <v>8</v>
+      </c>
+      <c r="C45" s="47"/>
+      <c r="D45" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="24">
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:H2"/>
@@ -2599,4 +3091,704 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C8A6E-862D-474B-ACCA-769FC441AECE}">
+  <dimension ref="A1:I44"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="55" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="25">
+        <v>8</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="25">
+        <v>2</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="25">
+        <v>5</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="25">
+        <v>5</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="25">
+        <v>5</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="25">
+        <v>5</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="25">
+        <v>9</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="25">
+        <v>9</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="25">
+        <v>9</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="25">
+        <v>9</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="30">
+        <v>3</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="33"/>
+      <c r="G15" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="30">
+        <v>3</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="33"/>
+      <c r="G16" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="30">
+        <v>3</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="30">
+        <v>10</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="H18" s="26"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+      <c r="B19" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="25">
+        <v>4</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="30">
+        <v>4</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="25" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="8">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="1">
+        <v>7</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="1">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="1">
+        <v>7</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="1">
+        <v>7</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="1">
+        <v>7</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="1">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="1">
+        <v>7</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="1">
+        <v>7</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>